<commit_message>
Get a valid Constellation name from the User to show the date asked by the user.
See: #2
</commit_message>
<xml_diff>
--- a/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
+++ b/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435148858654bebf/Documentos/Enciso Systems/GaN/GaN/Activity_Guide_Changes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C6C01E-4379-4D00-9311-E6D1EA784D87}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6322B63B-782D-4034-8F26-D6DE389C181B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Constellations</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>October 8-17, November 7-16</t>
+  </si>
+  <si>
+    <t>LEO</t>
   </si>
 </sst>
 </file>
@@ -179,24 +182,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -289,6 +274,24 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{D23468CE-86AC-4B82-B31C-E92D53D715BA}"/>
@@ -305,22 +308,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{288F47E8-6C6C-44F9-BEC9-DF3E64C8D1B4}" name="North_cons" displayName="North_cons" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{288F47E8-6C6C-44F9-BEC9-DF3E64C8D1B4}" name="North_cons" displayName="North_cons" ref="A1:B10" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:B10" xr:uid="{288F47E8-6C6C-44F9-BEC9-DF3E64C8D1B4}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5C8CBBB4-8F2A-4588-8FAF-8B6CEC3C19FA}" name="Constellations" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{AC2C1813-6FC8-4CC9-85F9-1741DD7BAA82}" name="Dates" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{5C8CBBB4-8F2A-4588-8FAF-8B6CEC3C19FA}" name="Constellations" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{AC2C1813-6FC8-4CC9-85F9-1741DD7BAA82}" name="Dates" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7804C795-F27A-4A2F-9433-D856786EC4D6}" name="South_cons" displayName="South_cons" ref="A1:B12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7804C795-F27A-4A2F-9433-D856786EC4D6}" name="South_cons" displayName="South_cons" ref="A1:B12" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:B12" xr:uid="{7804C795-F27A-4A2F-9433-D856786EC4D6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{651BA2BE-5D7C-45BB-BC19-94E1C6050556}" name="Constellations" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F5B6B34A-6AC5-4232-A702-470B79129FA3}" name="Dates" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{651BA2BE-5D7C-45BB-BC19-94E1C6050556}" name="Constellations" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F5B6B34A-6AC5-4232-A702-470B79129FA3}" name="Dates" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -626,7 +629,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -669,7 +672,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
South Translations have been completed
See: #3
</commit_message>
<xml_diff>
--- a/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
+++ b/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435148858654bebf/Documentos/Enciso Systems/GaN/GaN/Activity_Guide_Changes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6322B63B-782D-4034-8F26-D6DE389C181B}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DACD4958-8C31-49A8-A206-ACF4A58FEF4F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2475" windowWidth="19440" windowHeight="10320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="North" sheetId="1" r:id="rId1"/>
@@ -88,43 +88,43 @@
     <t>June 13-22, July 12-21, August 10-19</t>
   </si>
   <si>
+    <t>Crux</t>
+  </si>
+  <si>
+    <t>April 14-23, May 14-23, June 13-22</t>
+  </si>
+  <si>
+    <t>June 13-22</t>
+  </si>
+  <si>
+    <t>Scorpius</t>
+  </si>
+  <si>
+    <t>July 12-21, August 10-19</t>
+  </si>
+  <si>
+    <t>July 12-21</t>
+  </si>
+  <si>
+    <t>Sagittarius</t>
+  </si>
+  <si>
+    <t>August 10-19, September 9-18</t>
+  </si>
+  <si>
+    <t>Grus</t>
+  </si>
+  <si>
+    <t>September 9-18, October 8-17, November 7-16, December 6-15</t>
+  </si>
+  <si>
+    <t>October 8-17, November 7-16</t>
+  </si>
+  <si>
+    <t>LEO</t>
+  </si>
+  <si>
     <t>Canis Major</t>
-  </si>
-  <si>
-    <t>Crux</t>
-  </si>
-  <si>
-    <t>April 14-23, May 14-23, June 13-22</t>
-  </si>
-  <si>
-    <t>June 13-22</t>
-  </si>
-  <si>
-    <t>Scorpius</t>
-  </si>
-  <si>
-    <t>July 12-21, August 10-19</t>
-  </si>
-  <si>
-    <t>July 12-21</t>
-  </si>
-  <si>
-    <t>Sagittarius</t>
-  </si>
-  <si>
-    <t>August 10-19, September 9-18</t>
-  </si>
-  <si>
-    <t>Grus</t>
-  </si>
-  <si>
-    <t>September 9-18, October 8-17, November 7-16, December 6-15</t>
-  </si>
-  <si>
-    <t>October 8-17, November 7-16</t>
-  </si>
-  <si>
-    <t>LEO</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -672,7 +672,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -779,10 +779,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,15 +798,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,23 +814,23 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organize the README file in order to finish the text translation project
See: #5
</commit_message>
<xml_diff>
--- a/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
+++ b/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435148858654bebf/Documentos/Enciso Systems/GaN/GaN/Activity_Guide_Changes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DACD4958-8C31-49A8-A206-ACF4A58FEF4F}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46760004-F814-49DC-993E-30FDB6A7DF94}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2475" windowWidth="19440" windowHeight="10320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,6 +310,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{288F47E8-6C6C-44F9-BEC9-DF3E64C8D1B4}" name="North_cons" displayName="North_cons" ref="A1:B10" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:B10" xr:uid="{288F47E8-6C6C-44F9-BEC9-DF3E64C8D1B4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
+    <sortCondition ref="A2:A10"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5C8CBBB4-8F2A-4588-8FAF-8B6CEC3C19FA}" name="Constellations" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{AC2C1813-6FC8-4CC9-85F9-1741DD7BAA82}" name="Dates" dataDxfId="3"/>
@@ -321,6 +324,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7804C795-F27A-4A2F-9433-D856786EC4D6}" name="South_cons" displayName="South_cons" ref="A1:B12" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:B12" xr:uid="{7804C795-F27A-4A2F-9433-D856786EC4D6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{651BA2BE-5D7C-45BB-BC19-94E1C6050556}" name="Constellations" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{F5B6B34A-6AC5-4232-A702-470B79129FA3}" name="Dates" dataDxfId="0"/>
@@ -629,7 +635,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -648,18 +654,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,26 +678,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -704,18 +710,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +742,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -755,66 +761,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -825,20 +831,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All translations has benn revised
See: #4
</commit_message>
<xml_diff>
--- a/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
+++ b/Activity_Guide_Changes/GaN_cons_and_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/435148858654bebf/Documentos/Enciso Systems/GaN/GaN/Activity_Guide_Changes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46760004-F814-49DC-993E-30FDB6A7DF94}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_CF6B36B9A251247FC39D9A123DE0CCD2378769C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65847C3F-5FDD-42D9-95C6-C7FA45B8FAEC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2475" windowWidth="19440" windowHeight="10320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="North" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Constellations</t>
   </si>
@@ -37,21 +37,12 @@
     <t>Perseus</t>
   </si>
   <si>
-    <t>January 16-25, November 7-16, December 6-15</t>
-  </si>
-  <si>
     <t>Taurus</t>
   </si>
   <si>
-    <t>January 16-25</t>
-  </si>
-  <si>
     <t>Gemini</t>
   </si>
   <si>
-    <t>February 14-23, March 14-24</t>
-  </si>
-  <si>
     <t>Leo</t>
   </si>
   <si>
@@ -61,70 +52,88 @@
     <t>Bootes</t>
   </si>
   <si>
-    <t>May 14-23, June 13-22, July 12-21</t>
-  </si>
-  <si>
     <t>Cygnus</t>
   </si>
   <si>
-    <t>August 10-19, September 9-18, October 8-17</t>
-  </si>
-  <si>
     <t>Pegasus</t>
   </si>
   <si>
-    <t xml:space="preserve">October 8-17, November 7-16, </t>
-  </si>
-  <si>
     <t>Orion</t>
   </si>
   <si>
-    <t>January 16-25, February 14-23, March 14-24</t>
-  </si>
-  <si>
     <t>Hercules</t>
   </si>
   <si>
-    <t>June 13-22, July 12-21, August 10-19</t>
-  </si>
-  <si>
     <t>Crux</t>
   </si>
   <si>
-    <t>April 14-23, May 14-23, June 13-22</t>
-  </si>
-  <si>
-    <t>June 13-22</t>
-  </si>
-  <si>
     <t>Scorpius</t>
   </si>
   <si>
-    <t>July 12-21, August 10-19</t>
-  </si>
-  <si>
-    <t>July 12-21</t>
-  </si>
-  <si>
     <t>Sagittarius</t>
   </si>
   <si>
-    <t>August 10-19, September 9-18</t>
-  </si>
-  <si>
     <t>Grus</t>
   </si>
   <si>
-    <t>September 9-18, October 8-17, November 7-16, December 6-15</t>
-  </si>
-  <si>
-    <t>October 8-17, November 7-16</t>
-  </si>
-  <si>
     <t>LEO</t>
   </si>
   <si>
     <t>Canis Major</t>
+  </si>
+  <si>
+    <t>June 13- June 22</t>
+  </si>
+  <si>
+    <t>February 14- February 23, March 14 - March 24</t>
+  </si>
+  <si>
+    <t>September 9- September 18, October 8- October 17, November 7- November 16, December 6 -December 15</t>
+  </si>
+  <si>
+    <t>July 12 - July 21</t>
+  </si>
+  <si>
+    <t>April 14- April 23, May 14 - May 23</t>
+  </si>
+  <si>
+    <t>January 16- January 25, February 14 -February 23, March 14 - March 24</t>
+  </si>
+  <si>
+    <t>October 8 - October 17, November 7 - November 16</t>
+  </si>
+  <si>
+    <t>August 10 - August 19, September 9 -September 18</t>
+  </si>
+  <si>
+    <t>July 12 - July 21, August 10 - August 19</t>
+  </si>
+  <si>
+    <t>January 16 - January 25</t>
+  </si>
+  <si>
+    <t>May 14 - May 23, June 13 - June 22, July 12 - July 21</t>
+  </si>
+  <si>
+    <t>August 10 - August 19, September 9 -September 18, October 8 - October 17</t>
+  </si>
+  <si>
+    <t>February 14 - February 23, March 14 - March 24</t>
+  </si>
+  <si>
+    <t>June 13 - June 22, July 12 - July 21, August 10 - August 19</t>
+  </si>
+  <si>
+    <t>January 16 - January 25, February 14 - February 23, March 14 - March 24</t>
+  </si>
+  <si>
+    <t>January 16 - January 25, November 7- November 16, December 6 - December 15</t>
+  </si>
+  <si>
+    <t>October 8 - October17, November 7 - November 16</t>
+  </si>
+  <si>
+    <t>April 14 - April 23,  May 14 - May 23, June 13 - June 22</t>
   </si>
 </sst>
 </file>
@@ -635,7 +644,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -654,74 +663,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -742,7 +751,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -761,90 +770,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>